<commit_message>
Finish drawings and export to DWG and STL
</commit_message>
<xml_diff>
--- a/SolidWorks/BOM.xlsx
+++ b/SolidWorks/BOM.xlsx
@@ -16,7 +16,7 @@
   </sheets>
   <calcPr calcId="152511"/>
   <customWorkbookViews>
-    <customWorkbookView name="Daniel Olsen - Personal View" guid="{CEEF6D97-E30D-4B40-B36F-7D4EC2AC4B7E}" mergeInterval="0" personalView="1" yWindow="269" windowWidth="1440" windowHeight="759" activeSheetId="1"/>
+    <customWorkbookView name="Daniel Olsen - Personal View" guid="{3562AF30-6B2C-4A1D-B012-3BA7602874B1}" mergeInterval="0" personalView="1" xWindow="-1914" yWindow="154" windowWidth="1440" windowHeight="759" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="42">
   <si>
     <t>ITEM NO.</t>
   </si>
@@ -41,7 +41,7 @@
     <t>QTY.</t>
   </si>
   <si>
-    <t>Assem2^Cabinet_Flat</t>
+    <t>SideLeft</t>
   </si>
   <si>
     <t xml:space="preserve">  Side</t>
@@ -65,7 +65,10 @@
     <t xml:space="preserve">  FrontTVCoverSupport</t>
   </si>
   <si>
-    <t>Assem3^Cabinet_Flat</t>
+    <t xml:space="preserve">  FrontBlock</t>
+  </si>
+  <si>
+    <t>SideRight</t>
   </si>
   <si>
     <t>MonitorShelf</t>
@@ -87,9 +90,6 @@
   </si>
   <si>
     <t>Back</t>
-  </si>
-  <si>
-    <t>FrontBlock</t>
   </si>
   <si>
     <t>Front</t>
@@ -151,20 +151,8 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">  jlf-tp-8yt-w_asm1</t>
-  </si>
-  <si>
-    <t>12.6.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    SANWA_JOYSTICK_3</t>
-  </si>
-  <si>
-    <t>12.6.2</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">    </t>
+    <r>
+      <t xml:space="preserve">  </t>
     </r>
     <r>
       <rPr>
@@ -182,54 +170,15 @@
         <rFont val="Century Gothic"/>
         <family val="2"/>
       </rPr>
-      <t>SSANWA_JOYSTICK_6</t>
-    </r>
-  </si>
-  <si>
-    <t>12.6.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    SANWA_JOYSTICK_2</t>
-  </si>
-  <si>
-    <t>12.6.4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    SANWA_JOYSTICK_5</t>
-  </si>
-  <si>
-    <t>12.6.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    GT-Y</t>
-  </si>
-  <si>
-    <t>12.6.6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    SANWA_JOYSTICK_0</t>
-  </si>
-  <si>
-    <t>12.6.7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    BALL</t>
-  </si>
-  <si>
-    <t>12.6.8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    DUSTER</t>
-  </si>
-  <si>
-    <t>12.6.9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    E</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">  </t>
+      <t>horizontal_button_NEW</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">    mswitch</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
     </r>
     <r>
       <rPr>
@@ -251,17 +200,8 @@
     </r>
   </si>
   <si>
-    <t>12.7.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    mswitch</t>
-  </si>
-  <si>
-    <t>12.7.2</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">    </t>
+    <r>
+      <t xml:space="preserve">  </t>
     </r>
     <r>
       <rPr>
@@ -279,7 +219,7 @@
         <rFont val="Century Gothic"/>
         <family val="2"/>
       </rPr>
-      <t>horizontal_button_NEW</t>
+      <t>ControlPanelTopCover</t>
     </r>
   </si>
   <si>
@@ -290,6 +230,27 @@
   </si>
   <si>
     <t>93604A713</t>
+  </si>
+  <si>
+    <t>CornerSupport</t>
+  </si>
+  <si>
+    <t>TVSupportBack</t>
+  </si>
+  <si>
+    <t>TVSupportBlock</t>
+  </si>
+  <si>
+    <t>TVSupportFront</t>
+  </si>
+  <si>
+    <t>Crossmember2x4x30.5</t>
+  </si>
+  <si>
+    <t>BackTop</t>
+  </si>
+  <si>
+    <t>Marquee</t>
   </si>
 </sst>
 </file>
@@ -362,8 +323,8 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{ABEDB60B-286E-49D1-ABEE-96990863E3D2}">
-  <header guid="{ABEDB60B-286E-49D1-ABEE-96990863E3D2}" dateTime="2015-04-23T12:10:24" maxSheetId="2" userName="Daniel Olsen" r:id="rId1">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{FE8BF9B8-1DED-49A7-903E-C0C63F8ECA27}">
+  <header guid="{FE8BF9B8-1DED-49A7-903E-C0C63F8ECA27}" dateTime="2015-04-30T01:58:38" maxSheetId="2" userName="Daniel Olsen" r:id="rId1">
     <sheetIdMap count="1">
       <sheetId val="1"/>
     </sheetIdMap>
@@ -642,7 +603,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D48"/>
+  <dimension ref="A1:D47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -681,9 +642,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>1.1000000000000001</v>
-      </c>
+      <c r="A3" s="1"/>
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
@@ -693,9 +652,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>1.2</v>
-      </c>
+      <c r="A4" s="1"/>
       <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
@@ -705,9 +662,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>1.3</v>
-      </c>
+      <c r="A5" s="1"/>
       <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
@@ -717,9 +672,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>1.4</v>
-      </c>
+      <c r="A6" s="1"/>
       <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
@@ -729,9 +682,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>1.5</v>
-      </c>
+      <c r="A7" s="1"/>
       <c r="B7" s="2" t="s">
         <v>9</v>
       </c>
@@ -741,9 +692,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>1.6</v>
-      </c>
+      <c r="A8" s="1"/>
       <c r="B8" s="2" t="s">
         <v>10</v>
       </c>
@@ -753,9 +702,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>1.7</v>
-      </c>
+      <c r="A9" s="1"/>
       <c r="B9" s="2" t="s">
         <v>11</v>
       </c>
@@ -765,9 +712,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>2</v>
-      </c>
+      <c r="A10" s="1"/>
       <c r="B10" s="2" t="s">
         <v>12</v>
       </c>
@@ -778,10 +723,10 @@
     </row>
     <row r="11" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>2.1</v>
+        <v>2</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1">
@@ -789,11 +734,9 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>2.2000000000000002</v>
-      </c>
+      <c r="A12" s="1"/>
       <c r="B12" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1">
@@ -801,11 +744,9 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>2.2999999999999998</v>
-      </c>
+      <c r="A13" s="1"/>
       <c r="B13" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1">
@@ -813,11 +754,9 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>2.4</v>
-      </c>
+      <c r="A14" s="1"/>
       <c r="B14" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1">
@@ -825,11 +764,9 @@
       </c>
     </row>
     <row r="15" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>2.5</v>
-      </c>
+      <c r="A15" s="1"/>
       <c r="B15" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1">
@@ -837,11 +774,9 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>2.6</v>
-      </c>
+      <c r="A16" s="1"/>
       <c r="B16" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1">
@@ -849,11 +784,9 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>2.7</v>
-      </c>
+      <c r="A17" s="1"/>
       <c r="B17" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1">
@@ -861,11 +794,9 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
-        <v>3</v>
-      </c>
+      <c r="A18" s="1"/>
       <c r="B18" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1">
@@ -873,11 +804,9 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
-        <v>4</v>
-      </c>
+      <c r="A19" s="1"/>
       <c r="B19" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1">
@@ -886,22 +815,22 @@
     </row>
     <row r="20" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1">
@@ -910,22 +839,22 @@
     </row>
     <row r="22" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1">
@@ -934,10 +863,10 @@
     </row>
     <row r="24" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1">
@@ -946,22 +875,22 @@
     </row>
     <row r="25" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="1">
@@ -970,10 +899,10 @@
     </row>
     <row r="27" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="1">
@@ -982,10 +911,10 @@
     </row>
     <row r="28" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>12.1</v>
+        <v>11</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1">
@@ -993,11 +922,9 @@
       </c>
     </row>
     <row r="29" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A29" s="1">
-        <v>12.2</v>
-      </c>
+      <c r="A29" s="1"/>
       <c r="B29" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="1">
@@ -1005,11 +932,9 @@
       </c>
     </row>
     <row r="30" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A30" s="1">
-        <v>12.3</v>
-      </c>
+      <c r="A30" s="1"/>
       <c r="B30" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C30" s="1"/>
       <c r="D30" s="1">
@@ -1017,155 +942,141 @@
       </c>
     </row>
     <row r="31" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
-        <v>12.4</v>
-      </c>
+      <c r="A31" s="1"/>
       <c r="B31" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C31" s="1"/>
       <c r="D31" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="51.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="1">
-        <v>12.5</v>
-      </c>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A32" s="1"/>
       <c r="B32" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C32" s="1"/>
       <c r="D32" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A33" s="1">
-        <v>12.6</v>
-      </c>
+    <row r="33" spans="1:4" ht="51.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="1"/>
       <c r="B33" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C33" s="1"/>
       <c r="D33" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>29</v>
-      </c>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="34.5" x14ac:dyDescent="0.25">
+      <c r="A34" s="1"/>
       <c r="B34" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C34" s="1"/>
       <c r="D34" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="34.5" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
-        <v>31</v>
-      </c>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A35" s="1"/>
       <c r="B35" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C35" s="1"/>
       <c r="D35" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
-        <v>33</v>
-      </c>
+    <row r="36" spans="1:4" ht="34.5" x14ac:dyDescent="0.25">
+      <c r="A36" s="1"/>
       <c r="B36" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C36" s="1"/>
       <c r="D36" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
-        <v>35</v>
-      </c>
+    <row r="37" spans="1:4" ht="34.5" x14ac:dyDescent="0.25">
+      <c r="A37" s="1"/>
       <c r="B37" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C37" s="1"/>
       <c r="D37" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
-        <v>37</v>
+      <c r="A38" s="1">
+        <v>12</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C38" s="1"/>
       <c r="D38" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
-        <v>39</v>
+      <c r="A39" s="1">
+        <v>13</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="C39" s="1"/>
       <c r="D39" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
-        <v>41</v>
+      <c r="A40" s="1">
+        <v>14</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="C40" s="1"/>
       <c r="D40" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
-        <v>43</v>
+      <c r="A41" s="1">
+        <v>15</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="C41" s="1"/>
       <c r="D41" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
-        <v>45</v>
+      <c r="A42" s="1">
+        <v>16</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="C42" s="1"/>
       <c r="D42" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="34.5" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
-        <v>12.7</v>
+        <v>17</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="C43" s="1"/>
       <c r="D43" s="1">
@@ -1173,68 +1084,56 @@
       </c>
     </row>
     <row r="44" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
-        <v>48</v>
+      <c r="A44" s="1">
+        <v>18</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="C44" s="1"/>
       <c r="D44" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="34.5" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
-        <v>50</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>19</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="C45" s="1"/>
       <c r="D45" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="C46" s="1"/>
       <c r="D46" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="C47" s="1"/>
       <c r="D47" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A48" s="1">
-        <v>15</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C48" s="1"/>
-      <c r="D48" s="1">
-        <v>2</v>
-      </c>
-    </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{CEEF6D97-E30D-4B40-B36F-7D4EC2AC4B7E}">
+    <customSheetView guid="{3562AF30-6B2C-4A1D-B012-3BA7602874B1}">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>

</xml_diff>